<commit_message>
feat: status updating of students
</commit_message>
<xml_diff>
--- a/server/scripts/phd.xlsx
+++ b/server/scripts/phd.xlsx
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1697" uniqueCount="743">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1713" uniqueCount="751">
   <si>
     <t>name</t>
   </si>
@@ -2307,6 +2307,30 @@
   </si>
   <si>
     <t>Sahoo@hyderabad.bits-pilani.ac.in</t>
+  </si>
+  <si>
+    <t>eee.temp@hyderabad.bits-pilani.ac.in</t>
+  </si>
+  <si>
+    <t>f20220607@hyderabad.bits-pilani.ac.in</t>
+  </si>
+  <si>
+    <t>sanchay</t>
+  </si>
+  <si>
+    <t>sanchay2357@gmail.com</t>
+  </si>
+  <si>
+    <t>mech.temp@hyderabad.bits-pilani.ac.in</t>
+  </si>
+  <si>
+    <t>mech temp</t>
+  </si>
+  <si>
+    <t>zas</t>
+  </si>
+  <si>
+    <t>eee</t>
   </si>
 </sst>
 </file>
@@ -2361,11 +2385,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2392,10 +2417,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:U157" totalsRowShown="0">
-  <autoFilter ref="A1:U157"/>
-  <sortState ref="A2:U157">
-    <sortCondition ref="T1:T157"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:U159" totalsRowShown="0">
+  <autoFilter ref="A1:U159"/>
+  <sortState ref="A2:U159">
+    <sortCondition ref="T1:T159"/>
   </sortState>
   <tableColumns count="21">
     <tableColumn id="1" name="name"/>
@@ -2420,7 +2445,7 @@
     <tableColumn id="20" name="Supervisor Name"/>
     <tableColumn id="21" name="supervisor email2"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -2683,10 +2708,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U157"/>
+  <dimension ref="A1:U159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L73" workbookViewId="0">
-      <selection activeCell="U30" sqref="U30"/>
+    <sheetView tabSelected="1" topLeftCell="C145" workbookViewId="0">
+      <selection activeCell="N158" sqref="N158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -10182,7 +10207,7 @@
       <c r="T154" s="1" t="s">
         <v>699</v>
       </c>
-      <c r="U154" s="1" t="s">
+      <c r="U154" s="4" t="s">
         <v>667</v>
       </c>
     </row>
@@ -10327,8 +10352,88 @@
       <c r="T157" s="1" t="s">
         <v>653</v>
       </c>
-      <c r="U157" s="1" t="s">
+      <c r="U157" s="4" t="s">
         <v>685</v>
+      </c>
+    </row>
+    <row r="158" spans="1:21" ht="15" customHeight="1">
+      <c r="A158" s="1" t="s">
+        <v>750</v>
+      </c>
+      <c r="B158" s="4" t="s">
+        <v>743</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D158" t="s">
+        <v>480</v>
+      </c>
+      <c r="E158" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="F158" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="G158" s="1">
+        <v>41320210415</v>
+      </c>
+      <c r="H158" s="1"/>
+      <c r="I158" s="2" t="s">
+        <v>685</v>
+      </c>
+      <c r="J158" s="2" t="s">
+        <v>685</v>
+      </c>
+      <c r="K158" t="b">
+        <v>1</v>
+      </c>
+      <c r="L158" s="3">
+        <v>44852</v>
+      </c>
+      <c r="M158" s="1"/>
+      <c r="N158" s="3"/>
+      <c r="O158" s="3"/>
+      <c r="P158" s="3"/>
+      <c r="Q158" s="3"/>
+      <c r="R158" s="3"/>
+      <c r="S158" s="3"/>
+      <c r="T158" s="1" t="s">
+        <v>745</v>
+      </c>
+      <c r="U158" s="4" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="159" spans="1:21" ht="15" customHeight="1">
+      <c r="A159" t="s">
+        <v>748</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>747</v>
+      </c>
+      <c r="E159" t="s">
+        <v>482</v>
+      </c>
+      <c r="I159" s="2"/>
+      <c r="J159" s="2"/>
+      <c r="K159" t="b">
+        <v>1</v>
+      </c>
+      <c r="L159" s="3">
+        <v>44852</v>
+      </c>
+      <c r="M159" t="s">
+        <v>715</v>
+      </c>
+      <c r="N159" s="3">
+        <v>44932</v>
+      </c>
+      <c r="T159" t="s">
+        <v>749</v>
+      </c>
+      <c r="U159" s="4" t="s">
+        <v>744</v>
       </c>
     </row>
   </sheetData>
@@ -10648,12 +10753,20 @@
     <hyperlink ref="J62" r:id="rId310"/>
     <hyperlink ref="J40" r:id="rId311"/>
     <hyperlink ref="J24" r:id="rId312"/>
+    <hyperlink ref="U157" r:id="rId313"/>
+    <hyperlink ref="U154" r:id="rId314"/>
+    <hyperlink ref="B159" r:id="rId315"/>
+    <hyperlink ref="I158" r:id="rId316"/>
+    <hyperlink ref="J158" r:id="rId317"/>
+    <hyperlink ref="U158" r:id="rId318"/>
+    <hyperlink ref="B158" r:id="rId319"/>
+    <hyperlink ref="U159" r:id="rId320"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <legacyDrawing r:id="rId313"/>
+  <legacyDrawing r:id="rId321"/>
   <tableParts count="1">
-    <tablePart r:id="rId314"/>
+    <tablePart r:id="rId322"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added test data for phd
</commit_message>
<xml_diff>
--- a/server/scripts/phd.xlsx
+++ b/server/scripts/phd.xlsx
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1697" uniqueCount="743">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1703" uniqueCount="747">
   <si>
     <t>name</t>
   </si>
@@ -2307,6 +2307,18 @@
   </si>
   <si>
     <t>Sahoo@hyderabad.bits-pilani.ac.in</t>
+  </si>
+  <si>
+    <t>eee temp</t>
+  </si>
+  <si>
+    <t>eee.temp@hyderabad.bits-pilani.ac.in</t>
+  </si>
+  <si>
+    <t>sanchay</t>
+  </si>
+  <si>
+    <t>f20220607@hyderabad.bits-pilani.ac.in</t>
   </si>
 </sst>
 </file>
@@ -2393,8 +2405,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:U157" totalsRowShown="0">
-  <autoFilter ref="A1:U157"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:U158" totalsRowShown="0">
+  <autoFilter ref="A1:U158"/>
   <sortState ref="A2:U159">
     <sortCondition ref="T1:T159"/>
   </sortState>
@@ -2684,10 +2696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U157"/>
+  <dimension ref="A1:U158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L145" workbookViewId="0">
-      <selection activeCell="Q164" sqref="Q164"/>
+    <sheetView tabSelected="1" topLeftCell="L148" workbookViewId="0">
+      <selection activeCell="U158" sqref="U158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -10330,6 +10342,37 @@
       </c>
       <c r="U157" s="4" t="s">
         <v>685</v>
+      </c>
+    </row>
+    <row r="158" spans="1:21" ht="15" customHeight="1">
+      <c r="A158" t="s">
+        <v>743</v>
+      </c>
+      <c r="B158" s="4" t="s">
+        <v>744</v>
+      </c>
+      <c r="D158" t="s">
+        <v>480</v>
+      </c>
+      <c r="E158" t="s">
+        <v>482</v>
+      </c>
+      <c r="F158">
+        <v>7990573763</v>
+      </c>
+      <c r="I158" s="2"/>
+      <c r="J158" s="2"/>
+      <c r="K158" t="b">
+        <v>1</v>
+      </c>
+      <c r="L158" s="3">
+        <v>44852</v>
+      </c>
+      <c r="T158" t="s">
+        <v>745</v>
+      </c>
+      <c r="U158" s="2" t="s">
+        <v>746</v>
       </c>
     </row>
   </sheetData>
@@ -10651,12 +10694,14 @@
     <hyperlink ref="J24" r:id="rId312"/>
     <hyperlink ref="U157" r:id="rId313"/>
     <hyperlink ref="U154" r:id="rId314"/>
+    <hyperlink ref="B158" r:id="rId315"/>
+    <hyperlink ref="U158" r:id="rId316"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <legacyDrawing r:id="rId315"/>
+  <legacyDrawing r:id="rId317"/>
   <tableParts count="1">
-    <tablePart r:id="rId316"/>
+    <tablePart r:id="rId318"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new pdf for updating backend changes for students proposal review
</commit_message>
<xml_diff>
--- a/server/scripts/phd.xlsx
+++ b/server/scripts/phd.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanch\OneDrive\Desktop\Erp\server\scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BITS EEE\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA9BC965-ACB7-444C-99A4-04FC9F937BE4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5844"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9405" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,12 +20,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>BITS EEE</author>
   </authors>
   <commentList>
-    <comment ref="O39" authorId="0" shapeId="0">
+    <comment ref="O39" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -49,7 +50,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K90" authorId="0" shapeId="0">
+    <comment ref="K90" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -2324,7 +2325,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -2405,33 +2406,33 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:U158" totalsRowShown="0">
-  <autoFilter ref="A1:U158"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:U158" totalsRowShown="0">
+  <autoFilter ref="A1:U158" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState ref="A2:U159">
     <sortCondition ref="T1:T159"/>
   </sortState>
   <tableColumns count="21">
-    <tableColumn id="1" name="name"/>
-    <tableColumn id="2" name="email"/>
-    <tableColumn id="3" name="bits id"/>
-    <tableColumn id="4" name="department(eee/mech)"/>
-    <tableColumn id="5" name="phd type(full time/ part time)"/>
-    <tableColumn id="6" name="phone number"/>
-    <tableColumn id="7" name="erp id"/>
-    <tableColumn id="8" name="personal email"/>
-    <tableColumn id="9" name="notional supervisor email" dataDxfId="1" dataCellStyle="Hyperlink"/>
-    <tableColumn id="10" name="supervisor email" dataDxfId="0" dataCellStyle="Hyperlink"/>
-    <tableColumn id="11" name="pas/fail the qe(true  or false)"/>
-    <tableColumn id="12" name="qualification date if passed"/>
-    <tableColumn id="13" name="Proposal Seminar"/>
-    <tableColumn id="14" name="Date of Proposal"/>
-    <tableColumn id="15" name="Presubmission Seminar"/>
-    <tableColumn id="16" name="Draft Notice"/>
-    <tableColumn id="17" name="Date of Presubmission"/>
-    <tableColumn id="18" name="Final Thesis"/>
-    <tableColumn id="19" name="Viva Voce"/>
-    <tableColumn id="20" name="Supervisor Name"/>
-    <tableColumn id="21" name="supervisor email2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="name"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="email"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="bits id"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="department(eee/mech)"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="phd type(full time/ part time)"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="phone number"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="erp id"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="personal email"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="notional supervisor email" dataDxfId="1" dataCellStyle="Hyperlink"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="supervisor email" dataDxfId="0" dataCellStyle="Hyperlink"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="pas/fail the qe(true  or false)"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="qualification date if passed"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Proposal Seminar"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Date of Proposal"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Presubmission Seminar"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Draft Notice"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Date of Presubmission"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Final Thesis"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Viva Voce"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Supervisor Name"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="supervisor email2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2695,35 +2696,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L148" workbookViewId="0">
-      <selection activeCell="U158" sqref="U158"/>
+    <sheetView tabSelected="1" topLeftCell="B43" workbookViewId="0">
+      <selection activeCell="L59" sqref="L59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.77734375" customWidth="1"/>
-    <col min="5" max="5" width="26.33203125" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" customWidth="1"/>
+    <col min="5" max="5" width="26.28515625" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
     <col min="7" max="7" width="12" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5546875" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="10.109375" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="11.109375" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="26" customWidth="1"/>
-    <col min="12" max="12" width="24.6640625" customWidth="1"/>
+    <col min="12" max="12" width="24.7109375" customWidth="1"/>
     <col min="13" max="13" width="17" customWidth="1"/>
-    <col min="14" max="14" width="16.5546875" customWidth="1"/>
-    <col min="15" max="15" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.6640625" customWidth="1"/>
+    <col min="14" max="14" width="16.5703125" customWidth="1"/>
+    <col min="15" max="15" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.7109375" customWidth="1"/>
     <col min="17" max="17" width="21" customWidth="1"/>
-    <col min="18" max="19" width="15.6640625" customWidth="1"/>
-    <col min="20" max="20" width="16.6640625" customWidth="1"/>
-    <col min="21" max="21" width="17.109375" customWidth="1"/>
+    <col min="18" max="19" width="15.7109375" customWidth="1"/>
+    <col min="20" max="20" width="16.7109375" customWidth="1"/>
+    <col min="21" max="21" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="14.25" customHeight="1">
@@ -2820,7 +2821,12 @@
       <c r="J2" s="2" t="s">
         <v>666</v>
       </c>
-      <c r="L2" s="1"/>
+      <c r="K2" t="b">
+        <v>1</v>
+      </c>
+      <c r="L2" s="3">
+        <v>45931</v>
+      </c>
       <c r="M2" s="1"/>
       <c r="T2" s="1" t="s">
         <v>704</v>
@@ -5052,7 +5058,12 @@
       <c r="J48" s="2" t="s">
         <v>656</v>
       </c>
-      <c r="L48" s="1"/>
+      <c r="K48" t="b">
+        <v>1</v>
+      </c>
+      <c r="L48" s="3">
+        <v>45931</v>
+      </c>
       <c r="M48" s="1"/>
       <c r="T48" s="1" t="s">
         <v>641</v>
@@ -5521,7 +5532,12 @@
       <c r="J58" s="2" t="s">
         <v>659</v>
       </c>
-      <c r="L58" s="1"/>
+      <c r="K58" t="b">
+        <v>1</v>
+      </c>
+      <c r="L58" s="3">
+        <v>45931</v>
+      </c>
       <c r="M58" s="1"/>
       <c r="T58" s="1" t="s">
         <v>642</v>
@@ -5665,7 +5681,12 @@
       <c r="J61" s="2" t="s">
         <v>673</v>
       </c>
-      <c r="L61" s="1"/>
+      <c r="K61" t="b">
+        <v>1</v>
+      </c>
+      <c r="L61" s="3">
+        <v>45931</v>
+      </c>
       <c r="M61" s="1"/>
       <c r="T61" s="1" t="s">
         <v>645</v>
@@ -7121,7 +7142,12 @@
       <c r="J91" s="2" t="s">
         <v>661</v>
       </c>
-      <c r="L91" s="1"/>
+      <c r="K91" t="b">
+        <v>1</v>
+      </c>
+      <c r="L91" s="3">
+        <v>45931</v>
+      </c>
       <c r="M91" s="1"/>
       <c r="T91" s="1" t="s">
         <v>643</v>
@@ -7159,7 +7185,12 @@
       <c r="J92" s="2" t="s">
         <v>661</v>
       </c>
-      <c r="L92" s="1"/>
+      <c r="K92" t="b">
+        <v>1</v>
+      </c>
+      <c r="L92" s="3">
+        <v>45931</v>
+      </c>
       <c r="M92" s="1"/>
       <c r="T92" s="1" t="s">
         <v>643</v>
@@ -10044,7 +10075,12 @@
       <c r="J151" s="2" t="s">
         <v>662</v>
       </c>
-      <c r="L151" s="1"/>
+      <c r="K151" t="b">
+        <v>1</v>
+      </c>
+      <c r="L151" s="3">
+        <v>45931</v>
+      </c>
       <c r="M151" s="1"/>
       <c r="T151" s="1" t="s">
         <v>697</v>
@@ -10380,322 +10416,322 @@
     <sortCondition ref="C2:C157"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="I49" r:id="rId1"/>
-    <hyperlink ref="I58" r:id="rId2"/>
-    <hyperlink ref="I66" r:id="rId3"/>
-    <hyperlink ref="I114" r:id="rId4"/>
-    <hyperlink ref="I115" r:id="rId5"/>
-    <hyperlink ref="I14" r:id="rId6"/>
-    <hyperlink ref="I88" r:id="rId7"/>
-    <hyperlink ref="I87" r:id="rId8"/>
-    <hyperlink ref="I44" r:id="rId9"/>
-    <hyperlink ref="I119" r:id="rId10"/>
-    <hyperlink ref="I106" r:id="rId11"/>
-    <hyperlink ref="I136" r:id="rId12"/>
-    <hyperlink ref="I118" r:id="rId13"/>
-    <hyperlink ref="I147" r:id="rId14"/>
-    <hyperlink ref="I132" r:id="rId15"/>
-    <hyperlink ref="I33" r:id="rId16"/>
-    <hyperlink ref="I102" r:id="rId17"/>
-    <hyperlink ref="I41" r:id="rId18"/>
-    <hyperlink ref="I3" r:id="rId19"/>
-    <hyperlink ref="I156" r:id="rId20"/>
-    <hyperlink ref="I96" r:id="rId21"/>
-    <hyperlink ref="I92" r:id="rId22"/>
-    <hyperlink ref="I7" r:id="rId23"/>
-    <hyperlink ref="I67" r:id="rId24"/>
-    <hyperlink ref="I61" r:id="rId25"/>
-    <hyperlink ref="I97" r:id="rId26"/>
-    <hyperlink ref="I54" r:id="rId27"/>
-    <hyperlink ref="I148" r:id="rId28"/>
-    <hyperlink ref="I64" r:id="rId29"/>
-    <hyperlink ref="I77" r:id="rId30"/>
-    <hyperlink ref="I76" r:id="rId31"/>
-    <hyperlink ref="I43" r:id="rId32"/>
-    <hyperlink ref="I4" r:id="rId33"/>
-    <hyperlink ref="I85" r:id="rId34"/>
-    <hyperlink ref="I74" r:id="rId35"/>
-    <hyperlink ref="I27" r:id="rId36"/>
-    <hyperlink ref="I117" r:id="rId37"/>
-    <hyperlink ref="I57" r:id="rId38"/>
-    <hyperlink ref="I73" r:id="rId39"/>
-    <hyperlink ref="I55" r:id="rId40"/>
-    <hyperlink ref="I143" r:id="rId41"/>
-    <hyperlink ref="I91" r:id="rId42"/>
-    <hyperlink ref="I141" r:id="rId43"/>
-    <hyperlink ref="I94" r:id="rId44"/>
-    <hyperlink ref="I18" r:id="rId45"/>
-    <hyperlink ref="I152" r:id="rId46"/>
-    <hyperlink ref="I2" r:id="rId47"/>
-    <hyperlink ref="I121" r:id="rId48"/>
-    <hyperlink ref="I47" r:id="rId49"/>
-    <hyperlink ref="I6" r:id="rId50"/>
-    <hyperlink ref="I17" r:id="rId51"/>
-    <hyperlink ref="I139" r:id="rId52"/>
-    <hyperlink ref="I130" r:id="rId53"/>
-    <hyperlink ref="I149" r:id="rId54"/>
-    <hyperlink ref="I35" r:id="rId55"/>
-    <hyperlink ref="I26" r:id="rId56"/>
-    <hyperlink ref="I100" r:id="rId57"/>
-    <hyperlink ref="I80" r:id="rId58"/>
-    <hyperlink ref="I142" r:id="rId59"/>
-    <hyperlink ref="I53" r:id="rId60"/>
-    <hyperlink ref="I122" r:id="rId61"/>
-    <hyperlink ref="I60" r:id="rId62"/>
-    <hyperlink ref="I111" r:id="rId63"/>
-    <hyperlink ref="I113" r:id="rId64"/>
-    <hyperlink ref="I99" r:id="rId65"/>
-    <hyperlink ref="I138" r:id="rId66"/>
-    <hyperlink ref="I29" r:id="rId67"/>
-    <hyperlink ref="I83" r:id="rId68"/>
-    <hyperlink ref="I134" r:id="rId69"/>
-    <hyperlink ref="I129" r:id="rId70"/>
-    <hyperlink ref="I153" r:id="rId71"/>
-    <hyperlink ref="I146" r:id="rId72"/>
-    <hyperlink ref="I82" r:id="rId73"/>
-    <hyperlink ref="I25" r:id="rId74"/>
-    <hyperlink ref="I81" r:id="rId75"/>
-    <hyperlink ref="I101" r:id="rId76"/>
-    <hyperlink ref="I21" r:id="rId77"/>
-    <hyperlink ref="I68" r:id="rId78"/>
-    <hyperlink ref="I11" r:id="rId79"/>
-    <hyperlink ref="I93" r:id="rId80"/>
-    <hyperlink ref="I50" r:id="rId81"/>
-    <hyperlink ref="I48" r:id="rId82"/>
-    <hyperlink ref="I15" r:id="rId83"/>
-    <hyperlink ref="I10" r:id="rId84"/>
-    <hyperlink ref="I151" r:id="rId85"/>
-    <hyperlink ref="I110" r:id="rId86"/>
-    <hyperlink ref="I38" r:id="rId87"/>
-    <hyperlink ref="I45" r:id="rId88"/>
-    <hyperlink ref="I37" r:id="rId89"/>
-    <hyperlink ref="I123" r:id="rId90"/>
-    <hyperlink ref="I103" r:id="rId91"/>
-    <hyperlink ref="I63" r:id="rId92"/>
-    <hyperlink ref="I133" r:id="rId93"/>
-    <hyperlink ref="I157" r:id="rId94"/>
-    <hyperlink ref="I30" r:id="rId95"/>
-    <hyperlink ref="I128" r:id="rId96"/>
-    <hyperlink ref="I124" r:id="rId97"/>
-    <hyperlink ref="I144" r:id="rId98"/>
-    <hyperlink ref="I12" r:id="rId99"/>
-    <hyperlink ref="I116" r:id="rId100"/>
-    <hyperlink ref="I20" r:id="rId101"/>
-    <hyperlink ref="I9" r:id="rId102"/>
-    <hyperlink ref="I140" r:id="rId103"/>
-    <hyperlink ref="I145" r:id="rId104"/>
-    <hyperlink ref="I72" r:id="rId105"/>
-    <hyperlink ref="I19" r:id="rId106"/>
-    <hyperlink ref="I8" r:id="rId107"/>
-    <hyperlink ref="I46" r:id="rId108"/>
-    <hyperlink ref="I125" r:id="rId109"/>
-    <hyperlink ref="I5" r:id="rId110"/>
-    <hyperlink ref="I155" r:id="rId111"/>
-    <hyperlink ref="I86" r:id="rId112"/>
-    <hyperlink ref="I36" r:id="rId113"/>
-    <hyperlink ref="I154" r:id="rId114"/>
-    <hyperlink ref="I42" r:id="rId115"/>
-    <hyperlink ref="I28" r:id="rId116"/>
-    <hyperlink ref="I70" r:id="rId117"/>
-    <hyperlink ref="I56" r:id="rId118"/>
-    <hyperlink ref="I13" r:id="rId119"/>
-    <hyperlink ref="I131" r:id="rId120"/>
-    <hyperlink ref="I23" r:id="rId121"/>
-    <hyperlink ref="I108" r:id="rId122"/>
-    <hyperlink ref="I59" r:id="rId123"/>
-    <hyperlink ref="I89" r:id="rId124"/>
-    <hyperlink ref="I150" r:id="rId125"/>
-    <hyperlink ref="I22" r:id="rId126"/>
-    <hyperlink ref="I75" r:id="rId127"/>
-    <hyperlink ref="I137" r:id="rId128"/>
-    <hyperlink ref="I52" r:id="rId129"/>
-    <hyperlink ref="I135" r:id="rId130"/>
-    <hyperlink ref="I51" r:id="rId131"/>
-    <hyperlink ref="I34" r:id="rId132"/>
-    <hyperlink ref="I39" r:id="rId133"/>
-    <hyperlink ref="I98" r:id="rId134"/>
-    <hyperlink ref="I127" r:id="rId135"/>
-    <hyperlink ref="I16" r:id="rId136"/>
-    <hyperlink ref="I69" r:id="rId137"/>
-    <hyperlink ref="I90" r:id="rId138"/>
-    <hyperlink ref="I95" r:id="rId139"/>
-    <hyperlink ref="I109" r:id="rId140"/>
-    <hyperlink ref="I65" r:id="rId141"/>
-    <hyperlink ref="I79" r:id="rId142"/>
-    <hyperlink ref="I71" r:id="rId143"/>
-    <hyperlink ref="I120" r:id="rId144"/>
-    <hyperlink ref="I126" r:id="rId145"/>
-    <hyperlink ref="I78" r:id="rId146"/>
-    <hyperlink ref="I112" r:id="rId147"/>
-    <hyperlink ref="I107" r:id="rId148"/>
-    <hyperlink ref="I32" r:id="rId149"/>
-    <hyperlink ref="I105" r:id="rId150"/>
-    <hyperlink ref="I31" r:id="rId151"/>
-    <hyperlink ref="I104" r:id="rId152"/>
-    <hyperlink ref="I84" r:id="rId153"/>
-    <hyperlink ref="I62" r:id="rId154"/>
-    <hyperlink ref="I40" r:id="rId155"/>
-    <hyperlink ref="I24" r:id="rId156"/>
-    <hyperlink ref="J49" r:id="rId157"/>
-    <hyperlink ref="J58" r:id="rId158"/>
-    <hyperlink ref="J66" r:id="rId159"/>
-    <hyperlink ref="J114" r:id="rId160"/>
-    <hyperlink ref="J115" r:id="rId161"/>
-    <hyperlink ref="J14" r:id="rId162"/>
-    <hyperlink ref="J88" r:id="rId163"/>
-    <hyperlink ref="J87" r:id="rId164"/>
-    <hyperlink ref="J44" r:id="rId165"/>
-    <hyperlink ref="J119" r:id="rId166"/>
-    <hyperlink ref="J106" r:id="rId167"/>
-    <hyperlink ref="J136" r:id="rId168"/>
-    <hyperlink ref="J118" r:id="rId169"/>
-    <hyperlink ref="J147" r:id="rId170"/>
-    <hyperlink ref="J132" r:id="rId171"/>
-    <hyperlink ref="J33" r:id="rId172"/>
-    <hyperlink ref="J102" r:id="rId173"/>
-    <hyperlink ref="J41" r:id="rId174"/>
-    <hyperlink ref="J3" r:id="rId175"/>
-    <hyperlink ref="J156" r:id="rId176"/>
-    <hyperlink ref="J96" r:id="rId177"/>
-    <hyperlink ref="J92" r:id="rId178"/>
-    <hyperlink ref="J7" r:id="rId179"/>
-    <hyperlink ref="J67" r:id="rId180"/>
-    <hyperlink ref="J61" r:id="rId181"/>
-    <hyperlink ref="J97" r:id="rId182"/>
-    <hyperlink ref="J54" r:id="rId183"/>
-    <hyperlink ref="J148" r:id="rId184"/>
-    <hyperlink ref="J64" r:id="rId185"/>
-    <hyperlink ref="J77" r:id="rId186"/>
-    <hyperlink ref="J76" r:id="rId187"/>
-    <hyperlink ref="J43" r:id="rId188"/>
-    <hyperlink ref="J4" r:id="rId189"/>
-    <hyperlink ref="J85" r:id="rId190"/>
-    <hyperlink ref="J74" r:id="rId191"/>
-    <hyperlink ref="J27" r:id="rId192"/>
-    <hyperlink ref="J117" r:id="rId193"/>
-    <hyperlink ref="J57" r:id="rId194"/>
-    <hyperlink ref="J73" r:id="rId195"/>
-    <hyperlink ref="J55" r:id="rId196"/>
-    <hyperlink ref="J143" r:id="rId197"/>
-    <hyperlink ref="J91" r:id="rId198"/>
-    <hyperlink ref="J141" r:id="rId199"/>
-    <hyperlink ref="J94" r:id="rId200"/>
-    <hyperlink ref="J18" r:id="rId201"/>
-    <hyperlink ref="J152" r:id="rId202"/>
-    <hyperlink ref="J2" r:id="rId203"/>
-    <hyperlink ref="J121" r:id="rId204"/>
-    <hyperlink ref="J47" r:id="rId205"/>
-    <hyperlink ref="J6" r:id="rId206"/>
-    <hyperlink ref="J17" r:id="rId207"/>
-    <hyperlink ref="J139" r:id="rId208"/>
-    <hyperlink ref="J130" r:id="rId209"/>
-    <hyperlink ref="J149" r:id="rId210"/>
-    <hyperlink ref="J35" r:id="rId211"/>
-    <hyperlink ref="J26" r:id="rId212"/>
-    <hyperlink ref="J100" r:id="rId213"/>
-    <hyperlink ref="J80" r:id="rId214"/>
-    <hyperlink ref="J142" r:id="rId215"/>
-    <hyperlink ref="J53" r:id="rId216"/>
-    <hyperlink ref="J122" r:id="rId217"/>
-    <hyperlink ref="J60" r:id="rId218"/>
-    <hyperlink ref="J111" r:id="rId219"/>
-    <hyperlink ref="J113" r:id="rId220"/>
-    <hyperlink ref="J99" r:id="rId221"/>
-    <hyperlink ref="J138" r:id="rId222"/>
-    <hyperlink ref="J29" r:id="rId223"/>
-    <hyperlink ref="J83" r:id="rId224"/>
-    <hyperlink ref="J134" r:id="rId225"/>
-    <hyperlink ref="J129" r:id="rId226"/>
-    <hyperlink ref="J153" r:id="rId227"/>
-    <hyperlink ref="J146" r:id="rId228"/>
-    <hyperlink ref="J82" r:id="rId229"/>
-    <hyperlink ref="J25" r:id="rId230"/>
-    <hyperlink ref="J81" r:id="rId231"/>
-    <hyperlink ref="J101" r:id="rId232"/>
-    <hyperlink ref="J21" r:id="rId233"/>
-    <hyperlink ref="J68" r:id="rId234"/>
-    <hyperlink ref="J11" r:id="rId235"/>
-    <hyperlink ref="J93" r:id="rId236"/>
-    <hyperlink ref="J50" r:id="rId237"/>
-    <hyperlink ref="J48" r:id="rId238"/>
-    <hyperlink ref="J15" r:id="rId239"/>
-    <hyperlink ref="J10" r:id="rId240"/>
-    <hyperlink ref="J151" r:id="rId241"/>
-    <hyperlink ref="J110" r:id="rId242"/>
-    <hyperlink ref="J38" r:id="rId243"/>
-    <hyperlink ref="J45" r:id="rId244"/>
-    <hyperlink ref="J37" r:id="rId245"/>
-    <hyperlink ref="J123" r:id="rId246"/>
-    <hyperlink ref="J103" r:id="rId247"/>
-    <hyperlink ref="J63" r:id="rId248"/>
-    <hyperlink ref="J133" r:id="rId249"/>
-    <hyperlink ref="J157" r:id="rId250"/>
-    <hyperlink ref="J30" r:id="rId251"/>
-    <hyperlink ref="J128" r:id="rId252"/>
-    <hyperlink ref="J124" r:id="rId253"/>
-    <hyperlink ref="J144" r:id="rId254"/>
-    <hyperlink ref="J12" r:id="rId255"/>
-    <hyperlink ref="J116" r:id="rId256"/>
-    <hyperlink ref="J20" r:id="rId257"/>
-    <hyperlink ref="J9" r:id="rId258"/>
-    <hyperlink ref="J140" r:id="rId259"/>
-    <hyperlink ref="J145" r:id="rId260"/>
-    <hyperlink ref="J72" r:id="rId261"/>
-    <hyperlink ref="J19" r:id="rId262"/>
-    <hyperlink ref="J8" r:id="rId263"/>
-    <hyperlink ref="J46" r:id="rId264"/>
-    <hyperlink ref="J125" r:id="rId265"/>
-    <hyperlink ref="J5" r:id="rId266"/>
-    <hyperlink ref="J155" r:id="rId267"/>
-    <hyperlink ref="J86" r:id="rId268"/>
-    <hyperlink ref="J36" r:id="rId269"/>
-    <hyperlink ref="J154" r:id="rId270"/>
-    <hyperlink ref="J42" r:id="rId271"/>
-    <hyperlink ref="J28" r:id="rId272"/>
-    <hyperlink ref="J70" r:id="rId273"/>
-    <hyperlink ref="J56" r:id="rId274"/>
-    <hyperlink ref="J13" r:id="rId275"/>
-    <hyperlink ref="J131" r:id="rId276"/>
-    <hyperlink ref="J23" r:id="rId277"/>
-    <hyperlink ref="J108" r:id="rId278"/>
-    <hyperlink ref="J59" r:id="rId279"/>
-    <hyperlink ref="J89" r:id="rId280"/>
-    <hyperlink ref="J150" r:id="rId281"/>
-    <hyperlink ref="J22" r:id="rId282"/>
-    <hyperlink ref="J75" r:id="rId283"/>
-    <hyperlink ref="J137" r:id="rId284"/>
-    <hyperlink ref="J52" r:id="rId285"/>
-    <hyperlink ref="J135" r:id="rId286"/>
-    <hyperlink ref="J51" r:id="rId287"/>
-    <hyperlink ref="J34" r:id="rId288"/>
-    <hyperlink ref="J39" r:id="rId289"/>
-    <hyperlink ref="J98" r:id="rId290"/>
-    <hyperlink ref="J127" r:id="rId291"/>
-    <hyperlink ref="J16" r:id="rId292"/>
-    <hyperlink ref="J69" r:id="rId293"/>
-    <hyperlink ref="J90" r:id="rId294"/>
-    <hyperlink ref="J95" r:id="rId295"/>
-    <hyperlink ref="J109" r:id="rId296"/>
-    <hyperlink ref="J65" r:id="rId297"/>
-    <hyperlink ref="J79" r:id="rId298"/>
-    <hyperlink ref="J71" r:id="rId299"/>
-    <hyperlink ref="J120" r:id="rId300"/>
-    <hyperlink ref="J126" r:id="rId301"/>
-    <hyperlink ref="J78" r:id="rId302"/>
-    <hyperlink ref="J112" r:id="rId303"/>
-    <hyperlink ref="J107" r:id="rId304"/>
-    <hyperlink ref="J32" r:id="rId305"/>
-    <hyperlink ref="J105" r:id="rId306"/>
-    <hyperlink ref="J31" r:id="rId307"/>
-    <hyperlink ref="J104" r:id="rId308"/>
-    <hyperlink ref="J84" r:id="rId309"/>
-    <hyperlink ref="J62" r:id="rId310"/>
-    <hyperlink ref="J40" r:id="rId311"/>
-    <hyperlink ref="J24" r:id="rId312"/>
-    <hyperlink ref="U157" r:id="rId313"/>
-    <hyperlink ref="U154" r:id="rId314"/>
-    <hyperlink ref="B158" r:id="rId315"/>
-    <hyperlink ref="U158" r:id="rId316"/>
+    <hyperlink ref="I49" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="I58" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="I66" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="I114" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="I115" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="I14" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="I88" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="I87" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="I44" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="I119" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="I106" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="I136" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="I118" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="I147" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="I132" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="I33" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="I102" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="I41" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="I3" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="I156" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="I96" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="I92" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="I7" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="I67" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="I61" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="I97" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="I54" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="I148" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="I64" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="I77" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="I76" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="I43" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="I4" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="I85" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="I74" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="I27" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="I117" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="I57" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="I73" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="I55" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="I143" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="I91" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="I141" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="I94" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="I18" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="I152" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="I2" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="I121" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="I47" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="I6" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="I17" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="I139" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="I130" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="I149" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="I35" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="I26" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="I100" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="I80" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="I142" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="I53" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="I122" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="I60" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="I111" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="I113" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="I99" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="I138" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="I29" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="I83" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="I134" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="I129" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="I153" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="I146" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="I82" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="I25" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="I81" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="I101" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="I21" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="I68" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="I11" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="I93" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="I50" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="I48" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="I15" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="I10" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="I151" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="I110" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="I38" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="I45" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="I37" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="I123" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="I103" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="I63" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="I133" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="I157" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="I30" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="I128" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="I124" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="I144" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="I12" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="I116" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="I20" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="I9" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="I140" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="I145" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="I72" r:id="rId105" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
+    <hyperlink ref="I19" r:id="rId106" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="I8" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
+    <hyperlink ref="I46" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
+    <hyperlink ref="I125" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
+    <hyperlink ref="I5" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="I155" r:id="rId111" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="I86" r:id="rId112" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="I36" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
+    <hyperlink ref="I154" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
+    <hyperlink ref="I42" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
+    <hyperlink ref="I28" r:id="rId116" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="I70" r:id="rId117" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
+    <hyperlink ref="I56" r:id="rId118" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
+    <hyperlink ref="I13" r:id="rId119" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
+    <hyperlink ref="I131" r:id="rId120" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
+    <hyperlink ref="I23" r:id="rId121" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
+    <hyperlink ref="I108" r:id="rId122" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
+    <hyperlink ref="I59" r:id="rId123" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
+    <hyperlink ref="I89" r:id="rId124" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
+    <hyperlink ref="I150" r:id="rId125" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
+    <hyperlink ref="I22" r:id="rId126" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
+    <hyperlink ref="I75" r:id="rId127" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
+    <hyperlink ref="I137" r:id="rId128" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
+    <hyperlink ref="I52" r:id="rId129" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
+    <hyperlink ref="I135" r:id="rId130" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
+    <hyperlink ref="I51" r:id="rId131" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
+    <hyperlink ref="I34" r:id="rId132" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
+    <hyperlink ref="I39" r:id="rId133" xr:uid="{00000000-0004-0000-0000-000084000000}"/>
+    <hyperlink ref="I98" r:id="rId134" xr:uid="{00000000-0004-0000-0000-000085000000}"/>
+    <hyperlink ref="I127" r:id="rId135" xr:uid="{00000000-0004-0000-0000-000086000000}"/>
+    <hyperlink ref="I16" r:id="rId136" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
+    <hyperlink ref="I69" r:id="rId137" xr:uid="{00000000-0004-0000-0000-000088000000}"/>
+    <hyperlink ref="I90" r:id="rId138" xr:uid="{00000000-0004-0000-0000-000089000000}"/>
+    <hyperlink ref="I95" r:id="rId139" xr:uid="{00000000-0004-0000-0000-00008A000000}"/>
+    <hyperlink ref="I109" r:id="rId140" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
+    <hyperlink ref="I65" r:id="rId141" xr:uid="{00000000-0004-0000-0000-00008C000000}"/>
+    <hyperlink ref="I79" r:id="rId142" xr:uid="{00000000-0004-0000-0000-00008D000000}"/>
+    <hyperlink ref="I71" r:id="rId143" xr:uid="{00000000-0004-0000-0000-00008E000000}"/>
+    <hyperlink ref="I120" r:id="rId144" xr:uid="{00000000-0004-0000-0000-00008F000000}"/>
+    <hyperlink ref="I126" r:id="rId145" xr:uid="{00000000-0004-0000-0000-000090000000}"/>
+    <hyperlink ref="I78" r:id="rId146" xr:uid="{00000000-0004-0000-0000-000091000000}"/>
+    <hyperlink ref="I112" r:id="rId147" xr:uid="{00000000-0004-0000-0000-000092000000}"/>
+    <hyperlink ref="I107" r:id="rId148" xr:uid="{00000000-0004-0000-0000-000093000000}"/>
+    <hyperlink ref="I32" r:id="rId149" xr:uid="{00000000-0004-0000-0000-000094000000}"/>
+    <hyperlink ref="I105" r:id="rId150" xr:uid="{00000000-0004-0000-0000-000095000000}"/>
+    <hyperlink ref="I31" r:id="rId151" xr:uid="{00000000-0004-0000-0000-000096000000}"/>
+    <hyperlink ref="I104" r:id="rId152" xr:uid="{00000000-0004-0000-0000-000097000000}"/>
+    <hyperlink ref="I84" r:id="rId153" xr:uid="{00000000-0004-0000-0000-000098000000}"/>
+    <hyperlink ref="I62" r:id="rId154" xr:uid="{00000000-0004-0000-0000-000099000000}"/>
+    <hyperlink ref="I40" r:id="rId155" xr:uid="{00000000-0004-0000-0000-00009A000000}"/>
+    <hyperlink ref="I24" r:id="rId156" xr:uid="{00000000-0004-0000-0000-00009B000000}"/>
+    <hyperlink ref="J49" r:id="rId157" xr:uid="{00000000-0004-0000-0000-00009C000000}"/>
+    <hyperlink ref="J58" r:id="rId158" xr:uid="{00000000-0004-0000-0000-00009D000000}"/>
+    <hyperlink ref="J66" r:id="rId159" xr:uid="{00000000-0004-0000-0000-00009E000000}"/>
+    <hyperlink ref="J114" r:id="rId160" xr:uid="{00000000-0004-0000-0000-00009F000000}"/>
+    <hyperlink ref="J115" r:id="rId161" xr:uid="{00000000-0004-0000-0000-0000A0000000}"/>
+    <hyperlink ref="J14" r:id="rId162" xr:uid="{00000000-0004-0000-0000-0000A1000000}"/>
+    <hyperlink ref="J88" r:id="rId163" xr:uid="{00000000-0004-0000-0000-0000A2000000}"/>
+    <hyperlink ref="J87" r:id="rId164" xr:uid="{00000000-0004-0000-0000-0000A3000000}"/>
+    <hyperlink ref="J44" r:id="rId165" xr:uid="{00000000-0004-0000-0000-0000A4000000}"/>
+    <hyperlink ref="J119" r:id="rId166" xr:uid="{00000000-0004-0000-0000-0000A5000000}"/>
+    <hyperlink ref="J106" r:id="rId167" xr:uid="{00000000-0004-0000-0000-0000A6000000}"/>
+    <hyperlink ref="J136" r:id="rId168" xr:uid="{00000000-0004-0000-0000-0000A7000000}"/>
+    <hyperlink ref="J118" r:id="rId169" xr:uid="{00000000-0004-0000-0000-0000A8000000}"/>
+    <hyperlink ref="J147" r:id="rId170" xr:uid="{00000000-0004-0000-0000-0000A9000000}"/>
+    <hyperlink ref="J132" r:id="rId171" xr:uid="{00000000-0004-0000-0000-0000AA000000}"/>
+    <hyperlink ref="J33" r:id="rId172" xr:uid="{00000000-0004-0000-0000-0000AB000000}"/>
+    <hyperlink ref="J102" r:id="rId173" xr:uid="{00000000-0004-0000-0000-0000AC000000}"/>
+    <hyperlink ref="J41" r:id="rId174" xr:uid="{00000000-0004-0000-0000-0000AD000000}"/>
+    <hyperlink ref="J3" r:id="rId175" xr:uid="{00000000-0004-0000-0000-0000AE000000}"/>
+    <hyperlink ref="J156" r:id="rId176" xr:uid="{00000000-0004-0000-0000-0000AF000000}"/>
+    <hyperlink ref="J96" r:id="rId177" xr:uid="{00000000-0004-0000-0000-0000B0000000}"/>
+    <hyperlink ref="J92" r:id="rId178" xr:uid="{00000000-0004-0000-0000-0000B1000000}"/>
+    <hyperlink ref="J7" r:id="rId179" xr:uid="{00000000-0004-0000-0000-0000B2000000}"/>
+    <hyperlink ref="J67" r:id="rId180" xr:uid="{00000000-0004-0000-0000-0000B3000000}"/>
+    <hyperlink ref="J61" r:id="rId181" xr:uid="{00000000-0004-0000-0000-0000B4000000}"/>
+    <hyperlink ref="J97" r:id="rId182" xr:uid="{00000000-0004-0000-0000-0000B5000000}"/>
+    <hyperlink ref="J54" r:id="rId183" xr:uid="{00000000-0004-0000-0000-0000B6000000}"/>
+    <hyperlink ref="J148" r:id="rId184" xr:uid="{00000000-0004-0000-0000-0000B7000000}"/>
+    <hyperlink ref="J64" r:id="rId185" xr:uid="{00000000-0004-0000-0000-0000B8000000}"/>
+    <hyperlink ref="J77" r:id="rId186" xr:uid="{00000000-0004-0000-0000-0000B9000000}"/>
+    <hyperlink ref="J76" r:id="rId187" xr:uid="{00000000-0004-0000-0000-0000BA000000}"/>
+    <hyperlink ref="J43" r:id="rId188" xr:uid="{00000000-0004-0000-0000-0000BB000000}"/>
+    <hyperlink ref="J4" r:id="rId189" xr:uid="{00000000-0004-0000-0000-0000BC000000}"/>
+    <hyperlink ref="J85" r:id="rId190" xr:uid="{00000000-0004-0000-0000-0000BD000000}"/>
+    <hyperlink ref="J74" r:id="rId191" xr:uid="{00000000-0004-0000-0000-0000BE000000}"/>
+    <hyperlink ref="J27" r:id="rId192" xr:uid="{00000000-0004-0000-0000-0000BF000000}"/>
+    <hyperlink ref="J117" r:id="rId193" xr:uid="{00000000-0004-0000-0000-0000C0000000}"/>
+    <hyperlink ref="J57" r:id="rId194" xr:uid="{00000000-0004-0000-0000-0000C1000000}"/>
+    <hyperlink ref="J73" r:id="rId195" xr:uid="{00000000-0004-0000-0000-0000C2000000}"/>
+    <hyperlink ref="J55" r:id="rId196" xr:uid="{00000000-0004-0000-0000-0000C3000000}"/>
+    <hyperlink ref="J143" r:id="rId197" xr:uid="{00000000-0004-0000-0000-0000C4000000}"/>
+    <hyperlink ref="J91" r:id="rId198" xr:uid="{00000000-0004-0000-0000-0000C5000000}"/>
+    <hyperlink ref="J141" r:id="rId199" xr:uid="{00000000-0004-0000-0000-0000C6000000}"/>
+    <hyperlink ref="J94" r:id="rId200" xr:uid="{00000000-0004-0000-0000-0000C7000000}"/>
+    <hyperlink ref="J18" r:id="rId201" xr:uid="{00000000-0004-0000-0000-0000C8000000}"/>
+    <hyperlink ref="J152" r:id="rId202" xr:uid="{00000000-0004-0000-0000-0000C9000000}"/>
+    <hyperlink ref="J2" r:id="rId203" xr:uid="{00000000-0004-0000-0000-0000CA000000}"/>
+    <hyperlink ref="J121" r:id="rId204" xr:uid="{00000000-0004-0000-0000-0000CB000000}"/>
+    <hyperlink ref="J47" r:id="rId205" xr:uid="{00000000-0004-0000-0000-0000CC000000}"/>
+    <hyperlink ref="J6" r:id="rId206" xr:uid="{00000000-0004-0000-0000-0000CD000000}"/>
+    <hyperlink ref="J17" r:id="rId207" xr:uid="{00000000-0004-0000-0000-0000CE000000}"/>
+    <hyperlink ref="J139" r:id="rId208" xr:uid="{00000000-0004-0000-0000-0000CF000000}"/>
+    <hyperlink ref="J130" r:id="rId209" xr:uid="{00000000-0004-0000-0000-0000D0000000}"/>
+    <hyperlink ref="J149" r:id="rId210" xr:uid="{00000000-0004-0000-0000-0000D1000000}"/>
+    <hyperlink ref="J35" r:id="rId211" xr:uid="{00000000-0004-0000-0000-0000D2000000}"/>
+    <hyperlink ref="J26" r:id="rId212" xr:uid="{00000000-0004-0000-0000-0000D3000000}"/>
+    <hyperlink ref="J100" r:id="rId213" xr:uid="{00000000-0004-0000-0000-0000D4000000}"/>
+    <hyperlink ref="J80" r:id="rId214" xr:uid="{00000000-0004-0000-0000-0000D5000000}"/>
+    <hyperlink ref="J142" r:id="rId215" xr:uid="{00000000-0004-0000-0000-0000D6000000}"/>
+    <hyperlink ref="J53" r:id="rId216" xr:uid="{00000000-0004-0000-0000-0000D7000000}"/>
+    <hyperlink ref="J122" r:id="rId217" xr:uid="{00000000-0004-0000-0000-0000D8000000}"/>
+    <hyperlink ref="J60" r:id="rId218" xr:uid="{00000000-0004-0000-0000-0000D9000000}"/>
+    <hyperlink ref="J111" r:id="rId219" xr:uid="{00000000-0004-0000-0000-0000DA000000}"/>
+    <hyperlink ref="J113" r:id="rId220" xr:uid="{00000000-0004-0000-0000-0000DB000000}"/>
+    <hyperlink ref="J99" r:id="rId221" xr:uid="{00000000-0004-0000-0000-0000DC000000}"/>
+    <hyperlink ref="J138" r:id="rId222" xr:uid="{00000000-0004-0000-0000-0000DD000000}"/>
+    <hyperlink ref="J29" r:id="rId223" xr:uid="{00000000-0004-0000-0000-0000DE000000}"/>
+    <hyperlink ref="J83" r:id="rId224" xr:uid="{00000000-0004-0000-0000-0000DF000000}"/>
+    <hyperlink ref="J134" r:id="rId225" xr:uid="{00000000-0004-0000-0000-0000E0000000}"/>
+    <hyperlink ref="J129" r:id="rId226" xr:uid="{00000000-0004-0000-0000-0000E1000000}"/>
+    <hyperlink ref="J153" r:id="rId227" xr:uid="{00000000-0004-0000-0000-0000E2000000}"/>
+    <hyperlink ref="J146" r:id="rId228" xr:uid="{00000000-0004-0000-0000-0000E3000000}"/>
+    <hyperlink ref="J82" r:id="rId229" xr:uid="{00000000-0004-0000-0000-0000E4000000}"/>
+    <hyperlink ref="J25" r:id="rId230" xr:uid="{00000000-0004-0000-0000-0000E5000000}"/>
+    <hyperlink ref="J81" r:id="rId231" xr:uid="{00000000-0004-0000-0000-0000E6000000}"/>
+    <hyperlink ref="J101" r:id="rId232" xr:uid="{00000000-0004-0000-0000-0000E7000000}"/>
+    <hyperlink ref="J21" r:id="rId233" xr:uid="{00000000-0004-0000-0000-0000E8000000}"/>
+    <hyperlink ref="J68" r:id="rId234" xr:uid="{00000000-0004-0000-0000-0000E9000000}"/>
+    <hyperlink ref="J11" r:id="rId235" xr:uid="{00000000-0004-0000-0000-0000EA000000}"/>
+    <hyperlink ref="J93" r:id="rId236" xr:uid="{00000000-0004-0000-0000-0000EB000000}"/>
+    <hyperlink ref="J50" r:id="rId237" xr:uid="{00000000-0004-0000-0000-0000EC000000}"/>
+    <hyperlink ref="J48" r:id="rId238" xr:uid="{00000000-0004-0000-0000-0000ED000000}"/>
+    <hyperlink ref="J15" r:id="rId239" xr:uid="{00000000-0004-0000-0000-0000EE000000}"/>
+    <hyperlink ref="J10" r:id="rId240" xr:uid="{00000000-0004-0000-0000-0000EF000000}"/>
+    <hyperlink ref="J151" r:id="rId241" xr:uid="{00000000-0004-0000-0000-0000F0000000}"/>
+    <hyperlink ref="J110" r:id="rId242" xr:uid="{00000000-0004-0000-0000-0000F1000000}"/>
+    <hyperlink ref="J38" r:id="rId243" xr:uid="{00000000-0004-0000-0000-0000F2000000}"/>
+    <hyperlink ref="J45" r:id="rId244" xr:uid="{00000000-0004-0000-0000-0000F3000000}"/>
+    <hyperlink ref="J37" r:id="rId245" xr:uid="{00000000-0004-0000-0000-0000F4000000}"/>
+    <hyperlink ref="J123" r:id="rId246" xr:uid="{00000000-0004-0000-0000-0000F5000000}"/>
+    <hyperlink ref="J103" r:id="rId247" xr:uid="{00000000-0004-0000-0000-0000F6000000}"/>
+    <hyperlink ref="J63" r:id="rId248" xr:uid="{00000000-0004-0000-0000-0000F7000000}"/>
+    <hyperlink ref="J133" r:id="rId249" xr:uid="{00000000-0004-0000-0000-0000F8000000}"/>
+    <hyperlink ref="J157" r:id="rId250" xr:uid="{00000000-0004-0000-0000-0000F9000000}"/>
+    <hyperlink ref="J30" r:id="rId251" xr:uid="{00000000-0004-0000-0000-0000FA000000}"/>
+    <hyperlink ref="J128" r:id="rId252" xr:uid="{00000000-0004-0000-0000-0000FB000000}"/>
+    <hyperlink ref="J124" r:id="rId253" xr:uid="{00000000-0004-0000-0000-0000FC000000}"/>
+    <hyperlink ref="J144" r:id="rId254" xr:uid="{00000000-0004-0000-0000-0000FD000000}"/>
+    <hyperlink ref="J12" r:id="rId255" xr:uid="{00000000-0004-0000-0000-0000FE000000}"/>
+    <hyperlink ref="J116" r:id="rId256" xr:uid="{00000000-0004-0000-0000-0000FF000000}"/>
+    <hyperlink ref="J20" r:id="rId257" xr:uid="{00000000-0004-0000-0000-000000010000}"/>
+    <hyperlink ref="J9" r:id="rId258" xr:uid="{00000000-0004-0000-0000-000001010000}"/>
+    <hyperlink ref="J140" r:id="rId259" xr:uid="{00000000-0004-0000-0000-000002010000}"/>
+    <hyperlink ref="J145" r:id="rId260" xr:uid="{00000000-0004-0000-0000-000003010000}"/>
+    <hyperlink ref="J72" r:id="rId261" xr:uid="{00000000-0004-0000-0000-000004010000}"/>
+    <hyperlink ref="J19" r:id="rId262" xr:uid="{00000000-0004-0000-0000-000005010000}"/>
+    <hyperlink ref="J8" r:id="rId263" xr:uid="{00000000-0004-0000-0000-000006010000}"/>
+    <hyperlink ref="J46" r:id="rId264" xr:uid="{00000000-0004-0000-0000-000007010000}"/>
+    <hyperlink ref="J125" r:id="rId265" xr:uid="{00000000-0004-0000-0000-000008010000}"/>
+    <hyperlink ref="J5" r:id="rId266" xr:uid="{00000000-0004-0000-0000-000009010000}"/>
+    <hyperlink ref="J155" r:id="rId267" xr:uid="{00000000-0004-0000-0000-00000A010000}"/>
+    <hyperlink ref="J86" r:id="rId268" xr:uid="{00000000-0004-0000-0000-00000B010000}"/>
+    <hyperlink ref="J36" r:id="rId269" xr:uid="{00000000-0004-0000-0000-00000C010000}"/>
+    <hyperlink ref="J154" r:id="rId270" xr:uid="{00000000-0004-0000-0000-00000D010000}"/>
+    <hyperlink ref="J42" r:id="rId271" xr:uid="{00000000-0004-0000-0000-00000E010000}"/>
+    <hyperlink ref="J28" r:id="rId272" xr:uid="{00000000-0004-0000-0000-00000F010000}"/>
+    <hyperlink ref="J70" r:id="rId273" xr:uid="{00000000-0004-0000-0000-000010010000}"/>
+    <hyperlink ref="J56" r:id="rId274" xr:uid="{00000000-0004-0000-0000-000011010000}"/>
+    <hyperlink ref="J13" r:id="rId275" xr:uid="{00000000-0004-0000-0000-000012010000}"/>
+    <hyperlink ref="J131" r:id="rId276" xr:uid="{00000000-0004-0000-0000-000013010000}"/>
+    <hyperlink ref="J23" r:id="rId277" xr:uid="{00000000-0004-0000-0000-000014010000}"/>
+    <hyperlink ref="J108" r:id="rId278" xr:uid="{00000000-0004-0000-0000-000015010000}"/>
+    <hyperlink ref="J59" r:id="rId279" xr:uid="{00000000-0004-0000-0000-000016010000}"/>
+    <hyperlink ref="J89" r:id="rId280" xr:uid="{00000000-0004-0000-0000-000017010000}"/>
+    <hyperlink ref="J150" r:id="rId281" xr:uid="{00000000-0004-0000-0000-000018010000}"/>
+    <hyperlink ref="J22" r:id="rId282" xr:uid="{00000000-0004-0000-0000-000019010000}"/>
+    <hyperlink ref="J75" r:id="rId283" xr:uid="{00000000-0004-0000-0000-00001A010000}"/>
+    <hyperlink ref="J137" r:id="rId284" xr:uid="{00000000-0004-0000-0000-00001B010000}"/>
+    <hyperlink ref="J52" r:id="rId285" xr:uid="{00000000-0004-0000-0000-00001C010000}"/>
+    <hyperlink ref="J135" r:id="rId286" xr:uid="{00000000-0004-0000-0000-00001D010000}"/>
+    <hyperlink ref="J51" r:id="rId287" xr:uid="{00000000-0004-0000-0000-00001E010000}"/>
+    <hyperlink ref="J34" r:id="rId288" xr:uid="{00000000-0004-0000-0000-00001F010000}"/>
+    <hyperlink ref="J39" r:id="rId289" xr:uid="{00000000-0004-0000-0000-000020010000}"/>
+    <hyperlink ref="J98" r:id="rId290" xr:uid="{00000000-0004-0000-0000-000021010000}"/>
+    <hyperlink ref="J127" r:id="rId291" xr:uid="{00000000-0004-0000-0000-000022010000}"/>
+    <hyperlink ref="J16" r:id="rId292" xr:uid="{00000000-0004-0000-0000-000023010000}"/>
+    <hyperlink ref="J69" r:id="rId293" xr:uid="{00000000-0004-0000-0000-000024010000}"/>
+    <hyperlink ref="J90" r:id="rId294" xr:uid="{00000000-0004-0000-0000-000025010000}"/>
+    <hyperlink ref="J95" r:id="rId295" xr:uid="{00000000-0004-0000-0000-000026010000}"/>
+    <hyperlink ref="J109" r:id="rId296" xr:uid="{00000000-0004-0000-0000-000027010000}"/>
+    <hyperlink ref="J65" r:id="rId297" xr:uid="{00000000-0004-0000-0000-000028010000}"/>
+    <hyperlink ref="J79" r:id="rId298" xr:uid="{00000000-0004-0000-0000-000029010000}"/>
+    <hyperlink ref="J71" r:id="rId299" xr:uid="{00000000-0004-0000-0000-00002A010000}"/>
+    <hyperlink ref="J120" r:id="rId300" xr:uid="{00000000-0004-0000-0000-00002B010000}"/>
+    <hyperlink ref="J126" r:id="rId301" xr:uid="{00000000-0004-0000-0000-00002C010000}"/>
+    <hyperlink ref="J78" r:id="rId302" xr:uid="{00000000-0004-0000-0000-00002D010000}"/>
+    <hyperlink ref="J112" r:id="rId303" xr:uid="{00000000-0004-0000-0000-00002E010000}"/>
+    <hyperlink ref="J107" r:id="rId304" xr:uid="{00000000-0004-0000-0000-00002F010000}"/>
+    <hyperlink ref="J32" r:id="rId305" xr:uid="{00000000-0004-0000-0000-000030010000}"/>
+    <hyperlink ref="J105" r:id="rId306" xr:uid="{00000000-0004-0000-0000-000031010000}"/>
+    <hyperlink ref="J31" r:id="rId307" xr:uid="{00000000-0004-0000-0000-000032010000}"/>
+    <hyperlink ref="J104" r:id="rId308" xr:uid="{00000000-0004-0000-0000-000033010000}"/>
+    <hyperlink ref="J84" r:id="rId309" xr:uid="{00000000-0004-0000-0000-000034010000}"/>
+    <hyperlink ref="J62" r:id="rId310" xr:uid="{00000000-0004-0000-0000-000035010000}"/>
+    <hyperlink ref="J40" r:id="rId311" xr:uid="{00000000-0004-0000-0000-000036010000}"/>
+    <hyperlink ref="J24" r:id="rId312" xr:uid="{00000000-0004-0000-0000-000037010000}"/>
+    <hyperlink ref="U157" r:id="rId313" xr:uid="{00000000-0004-0000-0000-000038010000}"/>
+    <hyperlink ref="U154" r:id="rId314" xr:uid="{00000000-0004-0000-0000-000039010000}"/>
+    <hyperlink ref="B158" r:id="rId315" xr:uid="{00000000-0004-0000-0000-00003A010000}"/>
+    <hyperlink ref="U158" r:id="rId316" xr:uid="{00000000-0004-0000-0000-00003B010000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>